<commit_message>
P4-2136 test data obfuscating exercise.
</commit_message>
<xml_diff>
--- a/localstack/geoamey_sample.xlsx
+++ b/localstack/geoamey_sample.xlsx
@@ -39,10 +39,10 @@
     <t xml:space="preserve">Price</t>
   </si>
   <si>
-    <t xml:space="preserve">HMP Bedford</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bedford County Court</t>
+    <t xml:space="preserve">HMP Fred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freds County Court</t>
   </si>
   <si>
     <t xml:space="preserve">JID ref.</t>
@@ -375,7 +375,7 @@
     <numFmt numFmtId="165" formatCode="&quot;JID_&quot;00000"/>
     <numFmt numFmtId="166" formatCode="\£#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -404,6 +404,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -543,7 +550,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -565,6 +572,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -708,7 +719,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -740,17 +751,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="n">
+      <c r="D2" s="7" t="n">
         <v>43</v>
       </c>
     </row>
@@ -9966,576 +9977,576 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="n">
+      <c r="A2" s="11" t="n">
         <v>30853</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="n">
+      <c r="A3" s="11" t="n">
         <v>36240</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="n">
+      <c r="A4" s="11" t="n">
         <v>31127</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="11" t="n">
         <v>37092</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="n">
+      <c r="A6" s="11" t="n">
         <v>30144</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="11" t="n">
         <v>30539</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="n">
+      <c r="A9" s="11" t="n">
         <v>32919</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="n">
+      <c r="A10" s="11" t="n">
         <v>31032</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="11" t="n">
         <v>31119</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="n">
+      <c r="A12" s="11" t="n">
         <v>31196</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="n">
+      <c r="A13" s="11" t="n">
         <v>31141</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="n">
+      <c r="A14" s="11" t="n">
         <v>30169</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="13" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="n">
+      <c r="A15" s="11" t="n">
         <v>30623</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="13" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="n">
+      <c r="A16" s="11" t="n">
         <v>30052</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="13" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="n">
+      <c r="A17" s="11" t="n">
         <v>30426</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="n">
+      <c r="A18" s="11" t="n">
         <v>30104</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="13" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="n">
+      <c r="A19" s="11" t="n">
         <v>32107</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="n">
+      <c r="A20" s="11" t="n">
         <v>31112</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="n">
+      <c r="A21" s="11" t="n">
         <v>30165</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="n">
+      <c r="A22" s="11" t="n">
         <v>30676</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="n">
+      <c r="A23" s="11" t="n">
         <v>30040</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="n">
+      <c r="A24" s="11" t="n">
         <v>30861</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10" t="n">
+      <c r="A26" s="11" t="n">
         <v>31201</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10" t="n">
+      <c r="A27" s="11" t="n">
         <v>37092</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10" t="n">
+      <c r="A28" s="11" t="n">
         <v>30143</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="13" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10" t="n">
+      <c r="A30" s="11" t="n">
         <v>36616</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="13" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="13" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10" t="n">
+      <c r="A32" s="11" t="n">
         <v>31365</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="13" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10" t="n">
+      <c r="A33" s="11" t="n">
         <v>31120</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="n">
+      <c r="A34" s="11" t="n">
         <v>31197</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="13" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="n">
+      <c r="A35" s="11" t="n">
         <v>31140</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="13" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="n">
+      <c r="A36" s="11" t="n">
         <v>33378</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="13" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="n">
+      <c r="A37" s="11" t="n">
         <v>33906</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="13" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="n">
+      <c r="A38" s="11" t="n">
         <v>31297</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="13" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="n">
+      <c r="A39" s="11" t="n">
         <v>30164</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="13" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="n">
+      <c r="A40" s="11" t="n">
         <v>30677</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="13" t="n">
+      <c r="A41" s="14" t="n">
         <v>30177</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="16" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>